<commit_message>
create PruebaService automatically using NestJS commands
</commit_message>
<xml_diff>
--- a/calculo.xlsx
+++ b/calculo.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\workspace\cursoNestJS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69828551-DD66-4214-8C91-008AAF7486E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,10 +42,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -91,14 +85,15 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -373,18 +368,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,9 +387,10 @@
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,7 +404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2025</v>
       </c>
@@ -423,7 +419,7 @@
         <v>1623500</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2026</v>
       </c>
@@ -438,12 +434,12 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <f>B3-B2</f>
         <v>327405</v>
@@ -460,13 +456,14 @@
         <f>(D3/D2)-1</f>
         <v>0.23190637511549128</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -476,7 +473,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -486,45 +483,49 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <f>B2*23%</f>
         <v>327405</v>
       </c>
-      <c r="C11" s="1">
-        <f>C2*0.25</f>
-        <v>50000</v>
-      </c>
+      <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <f>B7*0.23</f>
         <v>384100</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="6">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="5">
         <f>B7+B13</f>
         <v>2054100</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
         <f>B3+B8</f>
         <v>1997405</v>
       </c>
+      <c r="D16" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>